<commit_message>
docs: updated documentation and diagram
</commit_message>
<xml_diff>
--- a/Documents/Version2_evaluation/Draft_metadata_CoreGenericHealth_p2.xlsx
+++ b/Documents/Version2_evaluation/Draft_metadata_CoreGenericHealth_p2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13804CAC-FD12-418D-BD4E-0867C0002F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD269A5F-D925-4C16-B95C-6F721E674A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="481">
   <si>
     <t>Property label</t>
   </si>
@@ -1000,6 +1000,9 @@
     <t>The date the dataset distribution was issued.</t>
   </si>
   <si>
+    <t>The minimum time period resolvable in the dataset distribution.</t>
+  </si>
+  <si>
     <t>rights</t>
   </si>
   <si>
@@ -1046,9 +1049,6 @@
     </r>
   </si>
   <si>
-    <t>The minimum time period resolvable in the dataset distribution.</t>
-  </si>
-  <si>
     <t>A name given to the Distribution</t>
   </si>
   <si>
@@ -1353,9 +1353,6 @@
   </si>
   <si>
     <t>A licence under which the Data service is made available</t>
-  </si>
-  <si>
-    <t>temporal literal</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1437,6 +1434,9 @@
     <t>foaf:mbox</t>
   </si>
   <si>
+    <t>A unique identifier of the agent.</t>
+  </si>
+  <si>
     <t>HRI v1</t>
   </si>
   <si>
@@ -1479,7 +1479,10 @@
     <t>vcard:hasEmail</t>
   </si>
   <si>
-    <t>has name</t>
+    <t>formatted name</t>
+  </si>
+  <si>
+    <t>The full name of the contact point.</t>
   </si>
   <si>
     <t>vcard:fn</t>
@@ -2323,7 +2326,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2366,15 +2368,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -2386,6 +2380,15 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4156,8 +4159,8 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4612,92 +4615,92 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="72.75" customHeight="1">
-      <c r="A15" s="137" t="s">
+      <c r="A15" s="141" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="142" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="137" t="s">
+      <c r="C15" s="141" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="139" t="s">
+      <c r="E15" s="143" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="140" t="s">
+      <c r="F15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="140" t="s">
+      <c r="G15" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="141" t="s">
+      <c r="H15" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="142" t="s">
+      <c r="I15" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="143" t="s">
+      <c r="J15" s="140" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="137"/>
-      <c r="B16" s="138"/>
-      <c r="C16" s="137"/>
+      <c r="A16" s="141"/>
+      <c r="B16" s="142"/>
+      <c r="C16" s="141"/>
       <c r="D16" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="139"/>
-      <c r="F16" s="140"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="143"/>
+      <c r="E16" s="143"/>
+      <c r="F16" s="137"/>
+      <c r="G16" s="137"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="139"/>
+      <c r="J16" s="140"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="137"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="137"/>
+      <c r="A17" s="141"/>
+      <c r="B17" s="142"/>
+      <c r="C17" s="141"/>
       <c r="D17" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="139"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="142"/>
-      <c r="J17" s="143"/>
+      <c r="E17" s="143"/>
+      <c r="F17" s="137"/>
+      <c r="G17" s="137"/>
+      <c r="H17" s="138"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="140"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="137"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="137"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="142"/>
+      <c r="C18" s="141"/>
       <c r="D18" s="114" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="139"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="142"/>
-      <c r="J18" s="143"/>
+      <c r="E18" s="143"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="139"/>
+      <c r="J18" s="140"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="137"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="137"/>
+      <c r="A19" s="141"/>
+      <c r="B19" s="142"/>
+      <c r="C19" s="141"/>
       <c r="D19" s="114" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="139"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="142"/>
-      <c r="J19" s="143"/>
+      <c r="E19" s="143"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="137"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="139"/>
+      <c r="J19" s="140"/>
     </row>
     <row r="20" spans="1:10" ht="43.5">
       <c r="A20" s="52" t="s">
@@ -4733,13 +4736,13 @@
       <c r="A21" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="134" t="s">
         <v>97</v>
       </c>
       <c r="C21" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="136" t="s">
+      <c r="D21" s="135" t="s">
         <v>99</v>
       </c>
       <c r="E21" s="10" t="s">
@@ -6010,13 +6013,13 @@
     </row>
     <row r="2" spans="1:10" ht="29.25">
       <c r="A2" s="100" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B2" s="88" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C2" s="76" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D2" s="75" t="s">
         <v>23</v>
@@ -6024,7 +6027,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="101"/>
       <c r="G2" s="100" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="H2" s="102" t="s">
         <v>62</v>
@@ -6038,13 +6041,13 @@
     </row>
     <row r="3" spans="1:10" ht="43.5">
       <c r="A3" s="104" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C3" s="82" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D3" s="81" t="s">
         <v>23</v>
@@ -6052,10 +6055,10 @@
       <c r="E3" s="83"/>
       <c r="F3" s="105"/>
       <c r="G3" s="106" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H3" s="81" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I3" s="106" t="s">
         <v>18</v>
@@ -6066,13 +6069,13 @@
     </row>
     <row r="4" spans="1:10" ht="43.5">
       <c r="A4" s="100" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B4" s="88" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C4" s="76" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D4" s="75" t="s">
         <v>23</v>
@@ -6080,10 +6083,10 @@
       <c r="E4" s="88"/>
       <c r="F4" s="101"/>
       <c r="G4" s="100" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H4" s="102" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="I4" s="103" t="s">
         <v>18</v>
@@ -6094,13 +6097,13 @@
     </row>
     <row r="5" spans="1:10" ht="43.5">
       <c r="A5" s="104" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C5" s="82" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D5" s="81" t="s">
         <v>23</v>
@@ -6110,10 +6113,10 @@
       </c>
       <c r="F5" s="105"/>
       <c r="G5" s="104" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="H5" s="81" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="I5" s="106" t="s">
         <v>18</v>
@@ -6124,13 +6127,13 @@
     </row>
     <row r="6" spans="1:10" ht="29.25">
       <c r="A6" s="100" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B6" s="110" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C6" s="76" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D6" s="75" t="s">
         <v>23</v>
@@ -6141,7 +6144,7 @@
         <v>140</v>
       </c>
       <c r="H6" s="102" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I6" s="103" t="s">
         <v>18</v>
@@ -6152,13 +6155,13 @@
     </row>
     <row r="7" spans="1:10" ht="43.5">
       <c r="A7" s="104" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C7" s="82" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D7" s="81" t="s">
         <v>23</v>
@@ -6180,23 +6183,23 @@
     </row>
     <row r="8" spans="1:10" ht="87">
       <c r="A8" s="100" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C8" s="76" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D8" s="75" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="108" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F8" s="80"/>
       <c r="G8" s="100" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="H8" s="102">
         <v>1</v>
@@ -6210,13 +6213,13 @@
     </row>
     <row r="9" spans="1:10" ht="29.25">
       <c r="A9" s="104" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B9" s="83" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C9" s="82" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D9" s="81" t="s">
         <v>23</v>
@@ -6224,7 +6227,7 @@
       <c r="E9" s="83"/>
       <c r="F9" s="105"/>
       <c r="G9" s="106" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H9" s="81" t="s">
         <v>62</v>
@@ -6238,13 +6241,13 @@
     </row>
     <row r="10" spans="1:10" ht="29.25">
       <c r="A10" s="100" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C10" s="76" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D10" s="75" t="s">
         <v>23</v>
@@ -6254,7 +6257,7 @@
       </c>
       <c r="F10" s="101"/>
       <c r="G10" s="100" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H10" s="102" t="s">
         <v>27</v>
@@ -6676,9 +6679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D216357D-42A4-49FA-9AEC-3DDC66FD6459}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="D2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7272,11 +7275,13 @@
       </c>
       <c r="K18" s="51"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="29.25">
       <c r="A19" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="B19" s="58"/>
+      <c r="B19" s="60" t="s">
+        <v>290</v>
+      </c>
       <c r="C19" s="57" t="s">
         <v>192</v>
       </c>
@@ -7301,25 +7306,25 @@
     </row>
     <row r="20" spans="1:11" ht="43.5">
       <c r="A20" s="52" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="53" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F20" s="66" t="s">
         <v>25</v>
       </c>
       <c r="G20" s="55" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H20" s="56" t="s">
         <v>62</v>
@@ -7337,16 +7342,16 @@
         <v>200</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C21" s="57" t="s">
         <v>202</v>
       </c>
       <c r="D21" s="111" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E21" s="60" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F21" s="61" t="s">
         <v>25</v>
@@ -7370,7 +7375,7 @@
         <v>207</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C22" s="52" t="s">
         <v>209</v>
@@ -7805,8 +7810,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8306,13 +8311,13 @@
     </row>
     <row r="17" spans="1:10" ht="29.25">
       <c r="A17" s="57" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B17" s="58" t="s">
         <v>332</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D17" s="57" t="s">
         <v>23</v>
@@ -9783,8 +9788,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="D21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9987,11 +9992,11 @@
     </row>
     <row r="7" spans="1:10" ht="60.75" customHeight="1">
       <c r="A7" s="57" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B7" s="58"/>
       <c r="C7" s="57" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D7" s="57" t="s">
         <v>23</v>
@@ -10327,7 +10332,7 @@
         <v>25</v>
       </c>
       <c r="G18" s="55" t="s">
-        <v>401</v>
+        <v>140</v>
       </c>
       <c r="H18" s="56" t="s">
         <v>62</v>
@@ -10369,10 +10374,10 @@
     </row>
     <row r="20" spans="1:10" ht="60.75" customHeight="1">
       <c r="A20" s="52" t="s">
+        <v>401</v>
+      </c>
+      <c r="B20" s="53" t="s">
         <v>402</v>
-      </c>
-      <c r="B20" s="53" t="s">
-        <v>403</v>
       </c>
       <c r="C20" s="52" t="s">
         <v>162</v>
@@ -10399,13 +10404,13 @@
     </row>
     <row r="21" spans="1:10" ht="60.75" customHeight="1">
       <c r="A21" s="57" t="s">
+        <v>403</v>
+      </c>
+      <c r="B21" s="58" t="s">
         <v>404</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="C21" s="57" t="s">
         <v>405</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>406</v>
       </c>
       <c r="D21" s="57" t="s">
         <v>23</v>
@@ -10429,10 +10434,10 @@
     </row>
     <row r="22" spans="1:10" ht="60.75" customHeight="1">
       <c r="A22" s="52" t="s">
+        <v>406</v>
+      </c>
+      <c r="B22" s="53" t="s">
         <v>407</v>
-      </c>
-      <c r="B22" s="53" t="s">
-        <v>408</v>
       </c>
       <c r="C22" s="52" t="s">
         <v>213</v>
@@ -10441,7 +10446,7 @@
         <v>23</v>
       </c>
       <c r="E22" s="65" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F22" s="67" t="s">
         <v>15</v>
@@ -10464,7 +10469,7 @@
         <v>216</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C23" s="59" t="s">
         <v>218</v>
@@ -10926,9 +10931,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F507EB-9201-48ED-BA4A-FAE0A681069A}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="D2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10979,16 +10984,16 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="75" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B2" s="76"/>
       <c r="C2" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="122" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="123"/>
+      <c r="D2" s="136" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="122"/>
       <c r="F2" s="78" t="s">
         <v>25</v>
       </c>
@@ -11005,13 +11010,13 @@
     </row>
     <row r="3" spans="1:10" ht="101.25">
       <c r="A3" s="81" t="s">
+        <v>411</v>
+      </c>
+      <c r="B3" s="82" t="s">
         <v>412</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="C3" s="81" t="s">
         <v>413</v>
-      </c>
-      <c r="C3" s="81" t="s">
-        <v>414</v>
       </c>
       <c r="D3" s="81" t="s">
         <v>23</v>
@@ -11037,7 +11042,9 @@
       <c r="A4" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="76"/>
+      <c r="B4" s="75" t="s">
+        <v>414</v>
+      </c>
       <c r="C4" s="75" t="s">
         <v>107</v>
       </c>
@@ -11062,28 +11069,28 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="29.25">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="123" t="s">
         <v>416</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="123" t="s">
         <v>418</v>
       </c>
       <c r="D5" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="125" t="s">
+      <c r="E5" s="124" t="s">
         <v>419</v>
       </c>
-      <c r="F5" s="126" t="s">
+      <c r="F5" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="126" t="s">
+      <c r="G5" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="127" t="s">
+      <c r="H5" s="126" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -11100,10 +11107,10 @@
       <c r="B6" s="76" t="s">
         <v>420</v>
       </c>
-      <c r="C6" s="130" t="s">
+      <c r="C6" s="129" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="131" t="s">
+      <c r="D6" s="130" t="s">
         <v>169</v>
       </c>
       <c r="E6" s="88" t="s">
@@ -11126,26 +11133,26 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="57.75">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="123" t="s">
         <v>422</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="C7" s="124" t="s">
+      <c r="C7" s="123" t="s">
         <v>318</v>
       </c>
-      <c r="D7" s="124" t="s">
+      <c r="D7" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="128"/>
-      <c r="F7" s="129" t="s">
+      <c r="E7" s="127"/>
+      <c r="F7" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="126" t="s">
+      <c r="G7" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="127" t="s">
+      <c r="H7" s="126" t="s">
         <v>62</v>
       </c>
       <c r="I7" s="6" t="s">
@@ -11771,7 +11778,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{66C46874-C442-43E5-AD72-76E8DA8688C4}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{7FCF1E17-4ED2-4EE1-ADC5-B09B88BC460F}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{039E290E-52BD-4FF4-8251-F25A3759F840}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11782,8 +11789,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="E2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11839,7 +11846,7 @@
       <c r="B2" s="76" t="s">
         <v>423</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="129" t="s">
         <v>425</v>
       </c>
       <c r="D2" s="75" t="s">
@@ -11872,7 +11879,7 @@
       <c r="C3" s="81" t="s">
         <v>428</v>
       </c>
-      <c r="D3" s="132" t="s">
+      <c r="D3" s="131" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="98"/>
@@ -11896,9 +11903,11 @@
       <c r="A4" s="75" t="s">
         <v>429</v>
       </c>
-      <c r="B4" s="76"/>
+      <c r="B4" s="76" t="s">
+        <v>430</v>
+      </c>
       <c r="C4" s="75" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D4" s="75" t="s">
         <v>23</v>
@@ -12632,10 +12641,10 @@
     </row>
     <row r="2" spans="1:10" ht="43.5">
       <c r="A2" s="76" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B2" s="94" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="96" t="s">
@@ -12646,7 +12655,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="97" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H2" s="80">
         <v>1</v>
@@ -12660,10 +12669,10 @@
     </row>
     <row r="3" spans="1:10" ht="72.75">
       <c r="A3" s="82" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B3" s="98" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C3" s="81"/>
       <c r="D3" s="83" t="s">
@@ -12674,7 +12683,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="85" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H3" s="87">
         <v>1</v>
@@ -13345,13 +13354,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="95" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>438</v>
-      </c>
-      <c r="C2" s="133" t="s">
         <v>439</v>
+      </c>
+      <c r="C2" s="132" t="s">
+        <v>440</v>
       </c>
       <c r="D2" s="95" t="s">
         <v>23</v>
@@ -13375,13 +13384,13 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="81" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B3" s="82" t="s">
-        <v>441</v>
-      </c>
-      <c r="C3" s="134" t="s">
         <v>442</v>
+      </c>
+      <c r="C3" s="133" t="s">
+        <v>443</v>
       </c>
       <c r="D3" s="81" t="s">
         <v>23</v>
@@ -13986,15 +13995,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
@@ -14006,7 +14006,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B1A1CF98C819F4881BB4349588D0C85" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff8ef391852eaca4511043a54bffd4a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfc87205-1831-4b6c-a7b4-76d40079a43e" xmlns:ns3="221af607-abea-4d5e-830c-567dcc03c0ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="201dd8b781da46d5daa37e3355db44fe" ns2:_="" ns3:_="">
     <xsd:import namespace="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
@@ -14249,14 +14249,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D613DAE5-7C40-407B-A7BA-7F08A27AA56E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D613DAE5-7C40-407B-A7BA-7F08A27AA56E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}"/>
 </file>
</xml_diff>

<commit_message>
docs: updated usage note for spatial
</commit_message>
<xml_diff>
--- a/Documents/Version2_evaluation/Draft_metadata_CoreGenericHealth_p2.xlsx
+++ b/Documents/Version2_evaluation/Draft_metadata_CoreGenericHealth_p2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD269A5F-D925-4C16-B95C-6F721E674A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97D0DB3C-C856-4F60-BF41-A67CD2C160D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="480">
   <si>
     <t>Property label</t>
   </si>
@@ -1085,304 +1085,301 @@
     <t>A free-text account of the Catalogue</t>
   </si>
   <si>
-    <t>A geographical area covered by the Catalogue</t>
+    <t>has part</t>
+  </si>
+  <si>
+    <t>A related Catalogue that is part of the described Catalogue</t>
+  </si>
+  <si>
+    <t>dct:hasPart</t>
+  </si>
+  <si>
+    <t>home page</t>
+  </si>
+  <si>
+    <t>A web page that acts as the main page for the Catalogue</t>
+  </si>
+  <si>
+    <t>foaf:homepage</t>
+  </si>
+  <si>
+    <t>foaf:Document</t>
+  </si>
+  <si>
+    <t>A language used in the textual metadata describing titles, descriptions, etc. of the Datasets in the Catalogue</t>
+  </si>
+  <si>
+    <t>dct:LinguisticSystem</t>
+  </si>
+  <si>
+    <t>licence</t>
+  </si>
+  <si>
+    <t>A licence under which the Catalogue can be used or reused.</t>
+  </si>
+  <si>
+    <t>dct:LicenseDocument</t>
+  </si>
+  <si>
+    <t>The most recent date on which the Catalogue was modified</t>
+  </si>
+  <si>
+    <t>An entity (organisation) responsible for making the Catalogue available</t>
+  </si>
+  <si>
+    <t>record</t>
+  </si>
+  <si>
+    <t>A Catalogue Record that is part of the Catalogue</t>
+  </si>
+  <si>
+    <t>dcat:record</t>
+  </si>
+  <si>
+    <t>dcat:CatalogRecord</t>
+  </si>
+  <si>
+    <t>The date of formal issuance (e.g., publication) of the Catalogue</t>
+  </si>
+  <si>
+    <t>A statement that specifies rights associated with the Catalogue</t>
+  </si>
+  <si>
+    <t>dct:RightsStatement</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>A site or end-point (Data Service) that is listed in the Catalogue</t>
+  </si>
+  <si>
+    <t>dcat:service</t>
+  </si>
+  <si>
+    <t>A temporal period that the Catalogue covers</t>
+  </si>
+  <si>
+    <t>themes</t>
+  </si>
+  <si>
+    <t>A knowledge organisation system used to classify the Catalogue's Datasets</t>
+  </si>
+  <si>
+    <t>dcat:themeTaxonomy</t>
+  </si>
+  <si>
+    <t>This property refers to a knowledge organisation system used to classify the Catalogue's Datasets. It must have at least the value NAL:data-theme as this is the mandatory controlled vocabulary for dcat:theme.</t>
+  </si>
+  <si>
+    <t>skos:ConceptScheme</t>
+  </si>
+  <si>
+    <t>A name given to the Catalogue</t>
+  </si>
+  <si>
+    <t>A name given to the Dataset Series.</t>
+  </si>
+  <si>
+    <t>This property can be repeated for parallel language versions of the name.</t>
+  </si>
+  <si>
+    <t>A free-text account of the Dataset Series.</t>
+  </si>
+  <si>
+    <t>This property can be repeated for parallel language versions. It is recommended to provide an indication about the dimensions the Dataset Series evolves.</t>
+  </si>
+  <si>
+    <t>relation</t>
+  </si>
+  <si>
+    <t>dct:relation</t>
+  </si>
+  <si>
+    <t>foaf:Project</t>
+  </si>
+  <si>
+    <t>xsd:string</t>
+  </si>
+  <si>
+    <t>creator name</t>
+  </si>
+  <si>
+    <t>The most recent date on which the Dataset Series was changed or modified</t>
+  </si>
+  <si>
+    <t>This is not equal to the most recent modified dataset in the collection of the dataset series.</t>
+  </si>
+  <si>
+    <t>The date of formal issuance (e.g., publication) of the Dataset Series</t>
+  </si>
+  <si>
+    <t>The moment when the dataset series was established as a managed resource. This is not equal to the release date of the oldest dataset in the collection of the dataset series.</t>
+  </si>
+  <si>
+    <t>An entity (organisation) responsible for ensuring the coherency of the Dataset Series</t>
+  </si>
+  <si>
+    <t>The publisher of the dataset series may not be the publisher of all datasets. E.g. a digital archive could take over the publishing of older datasets in the series.</t>
+  </si>
+  <si>
+    <t>Contact information that can be used for sending comments about the Dataset Series.</t>
+  </si>
+  <si>
+    <t>applicable legislation</t>
+  </si>
+  <si>
+    <t>The legislation that mandates the creation or management of the Dataset Series</t>
+  </si>
+  <si>
+    <t>The frequency at which the Dataset Series is updated</t>
+  </si>
+  <si>
+    <t>The frequency of a dataset series is not equal to the frequency of the dataset in the collection.</t>
+  </si>
+  <si>
+    <t>dct:Frequency</t>
+  </si>
+  <si>
+    <t>geographial coverage</t>
+  </si>
+  <si>
+    <t>A geographic region that is covered by the Dataset Series.</t>
+  </si>
+  <si>
+    <t>When spatial coverage is a dimension in the dataset series then the spatial coverage of each dataset in the collection should be part of the spatial coverage. In that case, an open ended value is recommended, e.g. EU or a broad bounding box covering the expected values.</t>
+  </si>
+  <si>
+    <t>dcatap:Location</t>
+  </si>
+  <si>
+    <t>A temporal period that the Dataset Series covers</t>
+  </si>
+  <si>
+    <t>When temporal coverage is a dimension in the dataset series then the temporal coverage of each dataset in the collection should be part of the temporal coverage. In that case, an open ended value is recommended, e.g. after 2012.</t>
+  </si>
+  <si>
+    <t>Access Rights</t>
+  </si>
+  <si>
+    <t>Information regarding access or restrictions based on privacy, security, or other policies</t>
+  </si>
+  <si>
+    <t>The legislation that mandates the creation or management of the Data Service</t>
+  </si>
+  <si>
+    <t>application profile</t>
+  </si>
+  <si>
+    <t>An established (technical) standard to which the Data Service conforms</t>
+  </si>
+  <si>
+    <t>The standards referred here SHOULD describe the Data Service and not the data it serves. The latter is provided by the dataset with which this Data Service is connected. For instance the data service adheres to the OGC WFS API standard, while the associated dataset adheres to the INSPIRE Address data model.</t>
+  </si>
+  <si>
+    <t>dct:Standard</t>
+  </si>
+  <si>
+    <t>Contact Point</t>
+  </si>
+  <si>
+    <t>Contact information that can be used for sending comments about the Data Service</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>A free-text account of the Data Service</t>
+  </si>
+  <si>
+    <t>end point description</t>
+  </si>
+  <si>
+    <t>A description of the services available via the end-points, including their operations, parameters etc.</t>
+  </si>
+  <si>
+    <t>dcat:endpointDescription</t>
+  </si>
+  <si>
+    <t>The property gives specific details of the actual endpoint instances, while dct:conformsTo is used to indicate the general standard or specification that the endpoints implement.</t>
+  </si>
+  <si>
+    <t>end point URL</t>
+  </si>
+  <si>
+    <t>The root location or primary endpoint of the service (an IRI).</t>
+  </si>
+  <si>
+    <t>dcat:endPointURL</t>
+  </si>
+  <si>
+    <t>The structure that can be returned by querying the endpointURL</t>
+  </si>
+  <si>
+    <t>dct:MediaTypeOrExtent</t>
+  </si>
+  <si>
+    <t>HVD Category</t>
+  </si>
+  <si>
+    <t>dcatap:hvdCategory</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>A keyword or tag describing the Data Service.</t>
+  </si>
+  <si>
+    <t>landing Page</t>
+  </si>
+  <si>
+    <t>A web page that provides access to the Data Service and/or additional information</t>
+  </si>
+  <si>
+    <t>dcat:landingPage</t>
+  </si>
+  <si>
+    <t>It is intended to point to a landing page at the original data service provider, not to a page on a site of a third party, such as an aggregator.</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>A licence under which the Data service is made available</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>An entity (organisation) responsible for making the Data Service available</t>
+  </si>
+  <si>
+    <t>serves dataset</t>
+  </si>
+  <si>
+    <t>This property refers to a collection of data that this data service can distribute</t>
+  </si>
+  <si>
+    <t>dcat:servesDataset</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>A category of the Data Service</t>
+  </si>
+  <si>
+    <t>A Data Service may be associated with multiple themes.</t>
+  </si>
+  <si>
+    <t>A name given to the Data Service.</t>
+  </si>
+  <si>
+    <t>country</t>
   </si>
   <si>
     <t>dct:Location</t>
-  </si>
-  <si>
-    <t>has part</t>
-  </si>
-  <si>
-    <t>A related Catalogue that is part of the described Catalogue</t>
-  </si>
-  <si>
-    <t>dct:hasPart</t>
-  </si>
-  <si>
-    <t>home page</t>
-  </si>
-  <si>
-    <t>A web page that acts as the main page for the Catalogue</t>
-  </si>
-  <si>
-    <t>foaf:homepage</t>
-  </si>
-  <si>
-    <t>foaf:Document</t>
-  </si>
-  <si>
-    <t>A language used in the textual metadata describing titles, descriptions, etc. of the Datasets in the Catalogue</t>
-  </si>
-  <si>
-    <t>dct:LinguisticSystem</t>
-  </si>
-  <si>
-    <t>licence</t>
-  </si>
-  <si>
-    <t>A licence under which the Catalogue can be used or reused.</t>
-  </si>
-  <si>
-    <t>dct:LicenseDocument</t>
-  </si>
-  <si>
-    <t>The most recent date on which the Catalogue was modified</t>
-  </si>
-  <si>
-    <t>An entity (organisation) responsible for making the Catalogue available</t>
-  </si>
-  <si>
-    <t>record</t>
-  </si>
-  <si>
-    <t>A Catalogue Record that is part of the Catalogue</t>
-  </si>
-  <si>
-    <t>dcat:record</t>
-  </si>
-  <si>
-    <t>dcat:CatalogRecord</t>
-  </si>
-  <si>
-    <t>The date of formal issuance (e.g., publication) of the Catalogue</t>
-  </si>
-  <si>
-    <t>A statement that specifies rights associated with the Catalogue</t>
-  </si>
-  <si>
-    <t>dct:RightsStatement</t>
-  </si>
-  <si>
-    <t>service</t>
-  </si>
-  <si>
-    <t>A site or end-point (Data Service) that is listed in the Catalogue</t>
-  </si>
-  <si>
-    <t>dcat:service</t>
-  </si>
-  <si>
-    <t>A temporal period that the Catalogue covers</t>
-  </si>
-  <si>
-    <t>themes</t>
-  </si>
-  <si>
-    <t>A knowledge organisation system used to classify the Catalogue's Datasets</t>
-  </si>
-  <si>
-    <t>dcat:themeTaxonomy</t>
-  </si>
-  <si>
-    <t>This property refers to a knowledge organisation system used to classify the Catalogue's Datasets. It must have at least the value NAL:data-theme as this is the mandatory controlled vocabulary for dcat:theme.</t>
-  </si>
-  <si>
-    <t>skos:ConceptScheme</t>
-  </si>
-  <si>
-    <t>A name given to the Catalogue</t>
-  </si>
-  <si>
-    <t>A name given to the Dataset Series.</t>
-  </si>
-  <si>
-    <t>This property can be repeated for parallel language versions of the name.</t>
-  </si>
-  <si>
-    <t>A free-text account of the Dataset Series.</t>
-  </si>
-  <si>
-    <t>This property can be repeated for parallel language versions. It is recommended to provide an indication about the dimensions the Dataset Series evolves.</t>
-  </si>
-  <si>
-    <t>relation</t>
-  </si>
-  <si>
-    <t>dct:relation</t>
-  </si>
-  <si>
-    <t>foaf:Project</t>
-  </si>
-  <si>
-    <t>xsd:string</t>
-  </si>
-  <si>
-    <t>creator name</t>
-  </si>
-  <si>
-    <t>The most recent date on which the Dataset Series was changed or modified</t>
-  </si>
-  <si>
-    <t>This is not equal to the most recent modified dataset in the collection of the dataset series.</t>
-  </si>
-  <si>
-    <t>The date of formal issuance (e.g., publication) of the Dataset Series</t>
-  </si>
-  <si>
-    <t>The moment when the dataset series was established as a managed resource. This is not equal to the release date of the oldest dataset in the collection of the dataset series.</t>
-  </si>
-  <si>
-    <t>An entity (organisation) responsible for ensuring the coherency of the Dataset Series</t>
-  </si>
-  <si>
-    <t>The publisher of the dataset series may not be the publisher of all datasets. E.g. a digital archive could take over the publishing of older datasets in the series.</t>
-  </si>
-  <si>
-    <t>Contact information that can be used for sending comments about the Dataset Series.</t>
-  </si>
-  <si>
-    <t>applicable legislation</t>
-  </si>
-  <si>
-    <t>The legislation that mandates the creation or management of the Dataset Series</t>
-  </si>
-  <si>
-    <t>The frequency at which the Dataset Series is updated</t>
-  </si>
-  <si>
-    <t>The frequency of a dataset series is not equal to the frequency of the dataset in the collection.</t>
-  </si>
-  <si>
-    <t>dct:Frequency</t>
-  </si>
-  <si>
-    <t>geographial coverage</t>
-  </si>
-  <si>
-    <t>A geographic region that is covered by the Dataset Series.</t>
-  </si>
-  <si>
-    <t>When spatial coverage is a dimension in the dataset series then the spatial coverage of each dataset in the collection should be part of the spatial coverage. In that case, an open ended value is recommended, e.g. EU or a broad bounding box covering the expected values.</t>
-  </si>
-  <si>
-    <t>dcatap:Location</t>
-  </si>
-  <si>
-    <t>A temporal period that the Dataset Series covers</t>
-  </si>
-  <si>
-    <t>When temporal coverage is a dimension in the dataset series then the temporal coverage of each dataset in the collection should be part of the temporal coverage. In that case, an open ended value is recommended, e.g. after 2012.</t>
-  </si>
-  <si>
-    <t>Access Rights</t>
-  </si>
-  <si>
-    <t>Information regarding access or restrictions based on privacy, security, or other policies</t>
-  </si>
-  <si>
-    <t>The legislation that mandates the creation or management of the Data Service</t>
-  </si>
-  <si>
-    <t>application profile</t>
-  </si>
-  <si>
-    <t>An established (technical) standard to which the Data Service conforms</t>
-  </si>
-  <si>
-    <t>The standards referred here SHOULD describe the Data Service and not the data it serves. The latter is provided by the dataset with which this Data Service is connected. For instance the data service adheres to the OGC WFS API standard, while the associated dataset adheres to the INSPIRE Address data model.</t>
-  </si>
-  <si>
-    <t>dct:Standard</t>
-  </si>
-  <si>
-    <t>Contact Point</t>
-  </si>
-  <si>
-    <t>Contact information that can be used for sending comments about the Data Service</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>A free-text account of the Data Service</t>
-  </si>
-  <si>
-    <t>end point description</t>
-  </si>
-  <si>
-    <t>A description of the services available via the end-points, including their operations, parameters etc.</t>
-  </si>
-  <si>
-    <t>dcat:endpointDescription</t>
-  </si>
-  <si>
-    <t>The property gives specific details of the actual endpoint instances, while dct:conformsTo is used to indicate the general standard or specification that the endpoints implement.</t>
-  </si>
-  <si>
-    <t>end point URL</t>
-  </si>
-  <si>
-    <t>The root location or primary endpoint of the service (an IRI).</t>
-  </si>
-  <si>
-    <t>dcat:endPointURL</t>
-  </si>
-  <si>
-    <t>The structure that can be returned by querying the endpointURL</t>
-  </si>
-  <si>
-    <t>dct:MediaTypeOrExtent</t>
-  </si>
-  <si>
-    <t>HVD Category</t>
-  </si>
-  <si>
-    <t>dcatap:hvdCategory</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>A keyword or tag describing the Data Service.</t>
-  </si>
-  <si>
-    <t>landing Page</t>
-  </si>
-  <si>
-    <t>A web page that provides access to the Data Service and/or additional information</t>
-  </si>
-  <si>
-    <t>dcat:landingPage</t>
-  </si>
-  <si>
-    <t>It is intended to point to a landing page at the original data service provider, not to a page on a site of a third party, such as an aggregator.</t>
-  </si>
-  <si>
-    <t>License</t>
-  </si>
-  <si>
-    <t>A licence under which the Data service is made available</t>
-  </si>
-  <si>
-    <t>Publisher</t>
-  </si>
-  <si>
-    <t>An entity (organisation) responsible for making the Data Service available</t>
-  </si>
-  <si>
-    <t>serves dataset</t>
-  </si>
-  <si>
-    <t>This property refers to a collection of data that this data service can distribute</t>
-  </si>
-  <si>
-    <t>dcat:servesDataset</t>
-  </si>
-  <si>
-    <t>Theme</t>
-  </si>
-  <si>
-    <t>A category of the Data Service</t>
-  </si>
-  <si>
-    <t>A Data Service may be associated with multiple themes.</t>
-  </si>
-  <si>
-    <t>A name given to the Data Service.</t>
-  </si>
-  <si>
-    <t>country</t>
   </si>
   <si>
     <t>email</t>
@@ -1963,7 +1960,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2390,12 +2387,37 @@
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="143">
+  <dxfs count="153">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -3063,6 +3085,106 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5875,42 +5997,42 @@
     <mergeCell ref="F15:F19"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:I1 F1:F15 F20:F57">
-    <cfRule type="cellIs" dxfId="142" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="15" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="16" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="17" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="18" operator="equal">
       <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H15 H20:H57">
-    <cfRule type="cellIs" dxfId="138" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="13" operator="greaterThan">
       <formula>"reviewd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="14" operator="equal">
       <formula>"needs review"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F15 F20:F57">
-    <cfRule type="cellIs" dxfId="136" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="4" operator="equal">
       <formula>"Not added"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J15 J20:J57">
-    <cfRule type="containsText" dxfId="135" priority="2" operator="containsText" text="HealthDCAT-AP">
+    <cfRule type="containsText" dxfId="145" priority="2" operator="containsText" text="HealthDCAT-AP">
       <formula>NOT(ISERROR(SEARCH("HealthDCAT-AP",J2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="3" operator="containsText" text="DCAT-AP NL">
+    <cfRule type="containsText" dxfId="144" priority="3" operator="containsText" text="DCAT-AP NL">
       <formula>NOT(ISERROR(SEARCH("DCAT-AP NL",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J15 J20:J57">
-    <cfRule type="containsText" dxfId="133" priority="1" operator="containsText" text="Health and NL">
+    <cfRule type="containsText" dxfId="143" priority="1" operator="containsText" text="Health and NL">
       <formula>NOT(ISERROR(SEARCH("Health and NL",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6013,13 +6135,13 @@
     </row>
     <row r="2" spans="1:10" ht="29.25">
       <c r="A2" s="100" t="s">
+        <v>443</v>
+      </c>
+      <c r="B2" s="88" t="s">
         <v>444</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="C2" s="76" t="s">
         <v>445</v>
-      </c>
-      <c r="C2" s="76" t="s">
-        <v>446</v>
       </c>
       <c r="D2" s="75" t="s">
         <v>23</v>
@@ -6027,7 +6149,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="101"/>
       <c r="G2" s="100" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H2" s="102" t="s">
         <v>62</v>
@@ -6041,13 +6163,13 @@
     </row>
     <row r="3" spans="1:10" ht="43.5">
       <c r="A3" s="104" t="s">
+        <v>447</v>
+      </c>
+      <c r="B3" s="83" t="s">
         <v>448</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="C3" s="82" t="s">
         <v>449</v>
-      </c>
-      <c r="C3" s="82" t="s">
-        <v>450</v>
       </c>
       <c r="D3" s="81" t="s">
         <v>23</v>
@@ -6055,10 +6177,10 @@
       <c r="E3" s="83"/>
       <c r="F3" s="105"/>
       <c r="G3" s="106" t="s">
+        <v>450</v>
+      </c>
+      <c r="H3" s="81" t="s">
         <v>451</v>
-      </c>
-      <c r="H3" s="81" t="s">
-        <v>452</v>
       </c>
       <c r="I3" s="106" t="s">
         <v>18</v>
@@ -6069,13 +6191,13 @@
     </row>
     <row r="4" spans="1:10" ht="43.5">
       <c r="A4" s="100" t="s">
+        <v>452</v>
+      </c>
+      <c r="B4" s="88" t="s">
         <v>453</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="C4" s="76" t="s">
         <v>454</v>
-      </c>
-      <c r="C4" s="76" t="s">
-        <v>455</v>
       </c>
       <c r="D4" s="75" t="s">
         <v>23</v>
@@ -6083,10 +6205,10 @@
       <c r="E4" s="88"/>
       <c r="F4" s="101"/>
       <c r="G4" s="100" t="s">
+        <v>455</v>
+      </c>
+      <c r="H4" s="102" t="s">
         <v>456</v>
-      </c>
-      <c r="H4" s="102" t="s">
-        <v>457</v>
       </c>
       <c r="I4" s="103" t="s">
         <v>18</v>
@@ -6097,13 +6219,13 @@
     </row>
     <row r="5" spans="1:10" ht="43.5">
       <c r="A5" s="104" t="s">
+        <v>457</v>
+      </c>
+      <c r="B5" s="83" t="s">
         <v>458</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="C5" s="82" t="s">
         <v>459</v>
-      </c>
-      <c r="C5" s="82" t="s">
-        <v>460</v>
       </c>
       <c r="D5" s="81" t="s">
         <v>23</v>
@@ -6113,10 +6235,10 @@
       </c>
       <c r="F5" s="105"/>
       <c r="G5" s="104" t="s">
+        <v>460</v>
+      </c>
+      <c r="H5" s="81" t="s">
         <v>461</v>
-      </c>
-      <c r="H5" s="81" t="s">
-        <v>462</v>
       </c>
       <c r="I5" s="106" t="s">
         <v>18</v>
@@ -6127,13 +6249,13 @@
     </row>
     <row r="6" spans="1:10" ht="29.25">
       <c r="A6" s="100" t="s">
+        <v>462</v>
+      </c>
+      <c r="B6" s="110" t="s">
         <v>463</v>
       </c>
-      <c r="B6" s="110" t="s">
+      <c r="C6" s="76" t="s">
         <v>464</v>
-      </c>
-      <c r="C6" s="76" t="s">
-        <v>465</v>
       </c>
       <c r="D6" s="75" t="s">
         <v>23</v>
@@ -6144,7 +6266,7 @@
         <v>140</v>
       </c>
       <c r="H6" s="102" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I6" s="103" t="s">
         <v>18</v>
@@ -6155,13 +6277,13 @@
     </row>
     <row r="7" spans="1:10" ht="43.5">
       <c r="A7" s="104" t="s">
+        <v>465</v>
+      </c>
+      <c r="B7" s="83" t="s">
         <v>466</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="C7" s="82" t="s">
         <v>467</v>
-      </c>
-      <c r="C7" s="82" t="s">
-        <v>468</v>
       </c>
       <c r="D7" s="81" t="s">
         <v>23</v>
@@ -6183,23 +6305,23 @@
     </row>
     <row r="8" spans="1:10" ht="87">
       <c r="A8" s="100" t="s">
+        <v>468</v>
+      </c>
+      <c r="B8" s="88" t="s">
         <v>469</v>
       </c>
-      <c r="B8" s="88" t="s">
+      <c r="C8" s="76" t="s">
         <v>470</v>
-      </c>
-      <c r="C8" s="76" t="s">
-        <v>471</v>
       </c>
       <c r="D8" s="75" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="108" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F8" s="80"/>
       <c r="G8" s="100" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H8" s="102">
         <v>1</v>
@@ -6213,13 +6335,13 @@
     </row>
     <row r="9" spans="1:10" ht="29.25">
       <c r="A9" s="104" t="s">
+        <v>473</v>
+      </c>
+      <c r="B9" s="83" t="s">
         <v>474</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="C9" s="82" t="s">
         <v>475</v>
-      </c>
-      <c r="C9" s="82" t="s">
-        <v>476</v>
       </c>
       <c r="D9" s="81" t="s">
         <v>23</v>
@@ -6227,7 +6349,7 @@
       <c r="E9" s="83"/>
       <c r="F9" s="105"/>
       <c r="G9" s="106" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H9" s="81" t="s">
         <v>62</v>
@@ -6241,23 +6363,23 @@
     </row>
     <row r="10" spans="1:10" ht="29.25">
       <c r="A10" s="100" t="s">
+        <v>477</v>
+      </c>
+      <c r="B10" s="109" t="s">
         <v>478</v>
       </c>
-      <c r="B10" s="109" t="s">
+      <c r="C10" s="76" t="s">
         <v>479</v>
-      </c>
-      <c r="C10" s="76" t="s">
-        <v>480</v>
       </c>
       <c r="D10" s="75" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="109" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F10" s="101"/>
       <c r="G10" s="100" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H10" s="102" t="s">
         <v>27</v>
@@ -7729,42 +7851,42 @@
     <sortCondition ref="A2:A23"/>
   </sortState>
   <conditionalFormatting sqref="H1:I1 F1:F53">
-    <cfRule type="cellIs" dxfId="132" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="7" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="8" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="9" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="10" operator="equal">
       <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H53">
-    <cfRule type="cellIs" dxfId="128" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="5" operator="greaterThan">
       <formula>"reviewd"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="6" operator="equal">
       <formula>"needs review"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F53">
-    <cfRule type="cellIs" dxfId="126" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="4" operator="equal">
       <formula>"Not added"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J53">
-    <cfRule type="containsText" dxfId="125" priority="2" operator="containsText" text="HealthDCAT-AP">
+    <cfRule type="containsText" dxfId="135" priority="2" operator="containsText" text="HealthDCAT-AP">
       <formula>NOT(ISERROR(SEARCH("HealthDCAT-AP",J2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="3" operator="containsText" text="DCAT-AP NL">
+    <cfRule type="containsText" dxfId="134" priority="3" operator="containsText" text="DCAT-AP NL">
       <formula>NOT(ISERROR(SEARCH("DCAT-AP NL",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J53">
-    <cfRule type="containsText" dxfId="123" priority="1" operator="containsText" text="Health and NL">
+    <cfRule type="containsText" dxfId="133" priority="1" operator="containsText" text="Health and NL">
       <formula>NOT(ISERROR(SEARCH("Health and NL",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7807,11 +7929,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD98AC81-9A7A-4660-B571-6D118AEA29BA}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8039,178 +8161,116 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="29.25">
-      <c r="A8" s="52" t="s">
+    <row r="8" spans="1:10" ht="15" customHeight="1">
+      <c r="A8" s="145" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="146" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="145" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="147" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="148" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="149" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="149" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="150" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="151" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="140" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1">
+      <c r="A9" s="145"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="145"/>
+      <c r="D9" s="152" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="148"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="150"/>
+      <c r="I9" s="151"/>
+      <c r="J9" s="140"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1">
+      <c r="A10" s="145"/>
+      <c r="B10" s="146"/>
+      <c r="C10" s="145"/>
+      <c r="D10" s="152" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="148"/>
+      <c r="F10" s="149"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="150"/>
+      <c r="I10" s="151"/>
+      <c r="J10" s="140"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1">
+      <c r="A11" s="145"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="152" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="148"/>
+      <c r="F11" s="149"/>
+      <c r="G11" s="149"/>
+      <c r="H11" s="150"/>
+      <c r="I11" s="151"/>
+      <c r="J11" s="140"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1">
+      <c r="A12" s="145"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="152" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="148"/>
+      <c r="F12" s="149"/>
+      <c r="G12" s="149"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="140"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1">
+      <c r="A13" s="57" t="s">
         <v>311</v>
       </c>
-      <c r="C8" s="52" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="66" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="55" t="s">
+      <c r="B13" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="H8" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="29.25">
-      <c r="A9" s="57" t="s">
+      <c r="C13" s="57" t="s">
         <v>313</v>
-      </c>
-      <c r="B9" s="58" t="s">
-        <v>314</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>315</v>
-      </c>
-      <c r="D9" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="60"/>
-      <c r="F9" s="117" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="62" t="s">
-        <v>304</v>
-      </c>
-      <c r="H9" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="29.25">
-      <c r="A10" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>317</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="72"/>
-      <c r="F10" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="55" t="s">
-        <v>319</v>
-      </c>
-      <c r="H10" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="43.5">
-      <c r="A11" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="58" t="s">
-        <v>320</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="111" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="118"/>
-      <c r="F11" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="62" t="s">
-        <v>321</v>
-      </c>
-      <c r="H11" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="29.25">
-      <c r="A12" s="52" t="s">
-        <v>322</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>323</v>
-      </c>
-      <c r="C12" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="D12" s="116" t="s">
-        <v>169</v>
-      </c>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="55" t="s">
-        <v>324</v>
-      </c>
-      <c r="H12" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="29.25">
-      <c r="A13" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="58" t="s">
-        <v>325</v>
-      </c>
-      <c r="C13" s="57" t="s">
-        <v>139</v>
       </c>
       <c r="D13" s="57" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="60"/>
-      <c r="F13" s="61" t="s">
+      <c r="F13" s="117" t="s">
         <v>25</v>
       </c>
       <c r="G13" s="62" t="s">
-        <v>140</v>
+        <v>304</v>
       </c>
       <c r="H13" s="63" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="I13" s="64" t="s">
         <v>18</v>
@@ -8219,55 +8279,55 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29.25">
+    <row r="14" spans="1:10" ht="15" customHeight="1">
       <c r="A14" s="52" t="s">
-        <v>160</v>
+        <v>314</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>326</v>
-      </c>
-      <c r="C14" s="69" t="s">
-        <v>162</v>
+        <v>315</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>316</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66" t="s">
-        <v>15</v>
+      <c r="E14" s="144"/>
+      <c r="F14" s="55" t="s">
+        <v>25</v>
       </c>
       <c r="G14" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="56">
-        <v>1</v>
+        <v>317</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>62</v>
       </c>
       <c r="I14" s="51" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="J14" s="51" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29.25">
+    <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="57" t="s">
-        <v>327</v>
+        <v>120</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>329</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="58"/>
-      <c r="F15" s="61" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="111" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="118"/>
+      <c r="F15" s="62" t="s">
         <v>25</v>
       </c>
       <c r="G15" s="62" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="H15" s="63" t="s">
         <v>27</v>
@@ -8279,25 +8339,25 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="29.25">
+    <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="52" t="s">
-        <v>187</v>
+        <v>320</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>331</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16" s="52" t="s">
-        <v>23</v>
+        <v>321</v>
+      </c>
+      <c r="C16" s="69" t="s">
+        <v>276</v>
+      </c>
+      <c r="D16" s="116" t="s">
+        <v>169</v>
       </c>
       <c r="E16" s="65"/>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="66" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="55" t="s">
-        <v>140</v>
+        <v>322</v>
       </c>
       <c r="H16" s="56" t="s">
         <v>62</v>
@@ -8311,23 +8371,23 @@
     </row>
     <row r="17" spans="1:10" ht="29.25">
       <c r="A17" s="57" t="s">
-        <v>291</v>
+        <v>137</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>293</v>
+        <v>139</v>
       </c>
       <c r="D17" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="68"/>
-      <c r="F17" s="62" t="s">
+      <c r="E17" s="60"/>
+      <c r="F17" s="61" t="s">
         <v>25</v>
       </c>
       <c r="G17" s="62" t="s">
-        <v>333</v>
+        <v>140</v>
       </c>
       <c r="H17" s="63" t="s">
         <v>62</v>
@@ -8341,29 +8401,29 @@
     </row>
     <row r="18" spans="1:10" ht="29.25">
       <c r="A18" s="52" t="s">
-        <v>334</v>
+        <v>160</v>
       </c>
       <c r="B18" s="53" t="s">
-        <v>335</v>
-      </c>
-      <c r="C18" s="52" t="s">
-        <v>336</v>
+        <v>324</v>
+      </c>
+      <c r="C18" s="69" t="s">
+        <v>162</v>
       </c>
       <c r="D18" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="55" t="s">
-        <v>25</v>
+      <c r="E18" s="65"/>
+      <c r="F18" s="66" t="s">
+        <v>15</v>
       </c>
       <c r="G18" s="55" t="s">
-        <v>240</v>
-      </c>
-      <c r="H18" s="56" t="s">
-        <v>27</v>
+        <v>57</v>
+      </c>
+      <c r="H18" s="56">
+        <v>1</v>
       </c>
       <c r="I18" s="51" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="J18" s="51" t="s">
         <v>69</v>
@@ -8371,23 +8431,23 @@
     </row>
     <row r="19" spans="1:10" ht="29.25">
       <c r="A19" s="57" t="s">
-        <v>204</v>
+        <v>325</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>206</v>
+        <v>327</v>
       </c>
       <c r="D19" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="118"/>
-      <c r="F19" s="62" t="s">
+      <c r="E19" s="58"/>
+      <c r="F19" s="61" t="s">
         <v>25</v>
       </c>
       <c r="G19" s="62" t="s">
-        <v>193</v>
+        <v>328</v>
       </c>
       <c r="H19" s="63" t="s">
         <v>27</v>
@@ -8399,30 +8459,28 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="57.75">
+    <row r="20" spans="1:10" ht="29.25">
       <c r="A20" s="52" t="s">
-        <v>338</v>
+        <v>187</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>339</v>
-      </c>
-      <c r="C20" s="69" t="s">
-        <v>340</v>
+        <v>329</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>189</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="65" t="s">
-        <v>341</v>
-      </c>
-      <c r="F20" s="66" t="s">
+      <c r="E20" s="65"/>
+      <c r="F20" s="67" t="s">
         <v>25</v>
       </c>
       <c r="G20" s="55" t="s">
-        <v>342</v>
+        <v>140</v>
       </c>
       <c r="H20" s="56" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="I20" s="51" t="s">
         <v>18</v>
@@ -8431,91 +8489,174 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" ht="29.25">
       <c r="A21" s="57" t="s">
-        <v>216</v>
+        <v>291</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="C21" s="57" t="s">
-        <v>218</v>
+        <v>293</v>
       </c>
       <c r="D21" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="61" t="s">
-        <v>15</v>
+      <c r="E21" s="68"/>
+      <c r="F21" s="62" t="s">
+        <v>25</v>
       </c>
       <c r="G21" s="62" t="s">
-        <v>68</v>
+        <v>331</v>
       </c>
       <c r="H21" s="63" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="I21" s="64" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="J21" s="51" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="52"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
+    <row r="22" spans="1:10" ht="29.25">
+      <c r="A22" s="52" t="s">
+        <v>332</v>
+      </c>
+      <c r="B22" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="C22" s="52" t="s">
+        <v>334</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="72"/>
+      <c r="F22" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="55" t="s">
+        <v>240</v>
+      </c>
+      <c r="H22" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29.25">
+      <c r="A23" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>335</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="118"/>
+      <c r="F23" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="62" t="s">
+        <v>193</v>
+      </c>
+      <c r="H23" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="57.75">
+      <c r="A24" s="52" t="s">
+        <v>336</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="C24" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>339</v>
+      </c>
+      <c r="F24" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="55" t="s">
+        <v>340</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="51" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="52"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="56"/>
+      <c r="A25" s="57" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25" s="58" t="s">
+        <v>341</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="60"/>
+      <c r="F25" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="51" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="52"/>
       <c r="B26" s="53"/>
       <c r="C26" s="52"/>
       <c r="D26" s="52"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="55"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
       <c r="G26" s="55"/>
       <c r="H26" s="56"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="52"/>
       <c r="B27" s="53"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="52"/>
-      <c r="E27" s="65"/>
+      <c r="E27" s="53"/>
       <c r="F27" s="66"/>
       <c r="G27" s="55"/>
       <c r="H27" s="56"/>
@@ -8526,7 +8667,7 @@
       <c r="C28" s="52"/>
       <c r="D28" s="52"/>
       <c r="E28" s="65"/>
-      <c r="F28" s="66"/>
+      <c r="F28" s="67"/>
       <c r="G28" s="55"/>
       <c r="H28" s="56"/>
     </row>
@@ -8535,8 +8676,8 @@
       <c r="B29" s="53"/>
       <c r="C29" s="52"/>
       <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="66"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="55"/>
       <c r="G29" s="55"/>
       <c r="H29" s="56"/>
     </row>
@@ -8544,19 +8685,18 @@
       <c r="A30" s="52"/>
       <c r="B30" s="53"/>
       <c r="C30" s="52"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="67"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="55"/>
       <c r="G30" s="55"/>
       <c r="H30" s="56"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="52"/>
       <c r="B31" s="53"/>
-      <c r="C31" s="52"/>
       <c r="D31" s="52"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="55"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="55"/>
       <c r="H31" s="56"/>
     </row>
@@ -8565,16 +8705,17 @@
       <c r="B32" s="53"/>
       <c r="C32" s="52"/>
       <c r="D32" s="52"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="55"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="55"/>
       <c r="H32" s="56"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="52"/>
       <c r="B33" s="53"/>
+      <c r="C33" s="52"/>
       <c r="D33" s="52"/>
-      <c r="E33" s="65"/>
+      <c r="E33" s="53"/>
       <c r="F33" s="66"/>
       <c r="G33" s="55"/>
       <c r="H33" s="56"/>
@@ -8583,9 +8724,9 @@
       <c r="A34" s="52"/>
       <c r="B34" s="53"/>
       <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
+      <c r="D34" s="73"/>
       <c r="E34" s="65"/>
-      <c r="F34" s="66"/>
+      <c r="F34" s="67"/>
       <c r="G34" s="55"/>
       <c r="H34" s="56"/>
     </row>
@@ -8594,8 +8735,8 @@
       <c r="B35" s="53"/>
       <c r="C35" s="52"/>
       <c r="D35" s="52"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="66"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="55"/>
       <c r="G35" s="55"/>
       <c r="H35" s="56"/>
     </row>
@@ -8604,18 +8745,17 @@
       <c r="B36" s="53"/>
       <c r="C36" s="52"/>
       <c r="D36" s="52"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="67"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="55"/>
       <c r="G36" s="55"/>
       <c r="H36" s="56"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="52"/>
       <c r="B37" s="53"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="55"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="55"/>
       <c r="H37" s="56"/>
     </row>
@@ -8664,16 +8804,17 @@
       <c r="B42" s="53"/>
       <c r="C42" s="52"/>
       <c r="D42" s="52"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="55"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="66"/>
       <c r="G42" s="55"/>
       <c r="H42" s="56"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="52"/>
       <c r="B43" s="53"/>
+      <c r="C43" s="52"/>
       <c r="D43" s="52"/>
-      <c r="E43" s="65"/>
+      <c r="E43" s="53"/>
       <c r="F43" s="66"/>
       <c r="G43" s="55"/>
       <c r="H43" s="56"/>
@@ -8684,7 +8825,7 @@
       <c r="C44" s="52"/>
       <c r="D44" s="52"/>
       <c r="E44" s="65"/>
-      <c r="F44" s="66"/>
+      <c r="F44" s="67"/>
       <c r="G44" s="55"/>
       <c r="H44" s="56"/>
     </row>
@@ -8692,9 +8833,9 @@
       <c r="A45" s="52"/>
       <c r="B45" s="53"/>
       <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="66"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="55"/>
       <c r="G45" s="55"/>
       <c r="H45" s="56"/>
     </row>
@@ -8703,18 +8844,17 @@
       <c r="B46" s="53"/>
       <c r="C46" s="52"/>
       <c r="D46" s="52"/>
-      <c r="E46" s="65"/>
-      <c r="F46" s="67"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="55"/>
       <c r="G46" s="55"/>
       <c r="H46" s="56"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="52"/>
       <c r="B47" s="53"/>
-      <c r="C47" s="52"/>
       <c r="D47" s="52"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="55"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="66"/>
       <c r="G47" s="55"/>
       <c r="H47" s="56"/>
     </row>
@@ -8723,8 +8863,8 @@
       <c r="B48" s="53"/>
       <c r="C48" s="52"/>
       <c r="D48" s="52"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="55"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="66"/>
       <c r="G48" s="55"/>
       <c r="H48" s="56"/>
     </row>
@@ -8734,7 +8874,7 @@
       <c r="C49" s="52"/>
       <c r="D49" s="52"/>
       <c r="E49" s="53"/>
-      <c r="F49" s="55"/>
+      <c r="F49" s="66"/>
       <c r="G49" s="55"/>
       <c r="H49" s="56"/>
     </row>
@@ -8742,18 +8882,19 @@
       <c r="A50" s="52"/>
       <c r="B50" s="53"/>
       <c r="C50" s="52"/>
-      <c r="D50" s="74"/>
+      <c r="D50" s="52"/>
       <c r="E50" s="65"/>
-      <c r="F50" s="55"/>
+      <c r="F50" s="67"/>
       <c r="G50" s="55"/>
       <c r="H50" s="56"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="52"/>
       <c r="B51" s="53"/>
+      <c r="C51" s="52"/>
       <c r="D51" s="52"/>
-      <c r="E51" s="65"/>
-      <c r="F51" s="66"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="55"/>
       <c r="G51" s="55"/>
       <c r="H51" s="56"/>
     </row>
@@ -8762,7 +8903,7 @@
       <c r="B52" s="53"/>
       <c r="C52" s="52"/>
       <c r="D52" s="52"/>
-      <c r="E52" s="65"/>
+      <c r="E52" s="53"/>
       <c r="F52" s="55"/>
       <c r="G52" s="55"/>
       <c r="H52" s="56"/>
@@ -8772,16 +8913,106 @@
       <c r="B53" s="53"/>
       <c r="C53" s="52"/>
       <c r="D53" s="52"/>
-      <c r="E53" s="65"/>
+      <c r="E53" s="53"/>
       <c r="F53" s="55"/>
       <c r="G53" s="55"/>
       <c r="H53" s="56"/>
     </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="52"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="56"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="52"/>
+      <c r="B55" s="53"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="66"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="56"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="52"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="56"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="52"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="65"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="56"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J21">
-    <sortCondition ref="A2:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J25">
+    <sortCondition ref="A2:A25"/>
   </sortState>
-  <conditionalFormatting sqref="H1:I1 F1:F53">
+  <mergeCells count="9">
+    <mergeCell ref="H8:H12"/>
+    <mergeCell ref="I8:I12"/>
+    <mergeCell ref="J8:J12"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="G8:G12"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H1:I1 F1:F7 F13:F57">
+    <cfRule type="cellIs" dxfId="132" priority="17" operator="equal">
+      <formula>"Optional"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="18" operator="equal">
+      <formula>"Recommended"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="19" operator="equal">
+      <formula>"Mandatory"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="20" operator="equal">
+      <formula>"Conditional"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H7 H13:H57">
+    <cfRule type="cellIs" dxfId="128" priority="15" operator="greaterThan">
+      <formula>"reviewd"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="16" operator="equal">
+      <formula>"needs review"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F7 F13:F57">
+    <cfRule type="cellIs" dxfId="126" priority="14" operator="equal">
+      <formula>"Not added"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J7 J13:J57">
+    <cfRule type="containsText" dxfId="125" priority="12" operator="containsText" text="HealthDCAT-AP">
+      <formula>NOT(ISERROR(SEARCH("HealthDCAT-AP",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="13" operator="containsText" text="DCAT-AP NL">
+      <formula>NOT(ISERROR(SEARCH("DCAT-AP NL",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J7 J13:J57">
+    <cfRule type="containsText" dxfId="123" priority="11" operator="containsText" text="Health and NL">
+      <formula>NOT(ISERROR(SEARCH("Health and NL",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
     <cfRule type="cellIs" dxfId="122" priority="7" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
@@ -8795,7 +9026,7 @@
       <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H53">
+  <conditionalFormatting sqref="H8">
     <cfRule type="cellIs" dxfId="118" priority="5" operator="greaterThan">
       <formula>"reviewd"</formula>
     </cfRule>
@@ -8803,50 +9034,55 @@
       <formula>"needs review"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F53">
+  <conditionalFormatting sqref="F8">
     <cfRule type="cellIs" dxfId="116" priority="4" operator="equal">
       <formula>"Not added"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J53">
+  <conditionalFormatting sqref="J8">
     <cfRule type="containsText" dxfId="115" priority="2" operator="containsText" text="HealthDCAT-AP">
-      <formula>NOT(ISERROR(SEARCH("HealthDCAT-AP",J2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HealthDCAT-AP",J8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="114" priority="3" operator="containsText" text="DCAT-AP NL">
-      <formula>NOT(ISERROR(SEARCH("DCAT-AP NL",J2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DCAT-AP NL",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J53">
+  <conditionalFormatting sqref="J8">
     <cfRule type="containsText" dxfId="113" priority="1" operator="containsText" text="Health and NL">
-      <formula>NOT(ISERROR(SEARCH("Health and NL",J2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Health and NL",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H47:H49 H24:H38 H2:H22" xr:uid="{2A32C7D3-75FA-463A-BF68-3B76762746E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H51:H53 H28:H42 H2:H8 H13:H26" xr:uid="{2A32C7D3-75FA-463A-BF68-3B76762746E5}">
       <formula1>"0..n, 0..1, 1, 1..n"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{5E2451C1-1FA6-42BF-907E-0BF14F90289A}">
       <formula1>"Mandatory, Recommended, Optional, Conditional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F49" xr:uid="{C9CBD033-88AB-4840-B5DC-D786E0636705}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J26:J1048576" xr:uid="{DF04DE99-7912-447A-8D69-145BAB6C72E0}">
+      <formula1>"DCAT-AP v3, HealthDCAT-AP, DCAT-AP NL, HRI v1"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1" xr:uid="{4FA88F03-C3E1-4A61-AEAF-7DC76A65E608}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8 F13:F53" xr:uid="{C9CBD033-88AB-4840-B5DC-D786E0636705}">
       <formula1>"Mandatory, Recommended, Optional, Conditional, Not added"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J22:J1048576" xr:uid="{DF04DE99-7912-447A-8D69-145BAB6C72E0}">
-      <formula1>"DCAT-AP v3, HealthDCAT-AP, DCAT-AP NL, HRI v1"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{BDB4FC21-78EB-412C-BDE7-A8B62BC5F962}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I8 I13:I1048576" xr:uid="{BDB4FC21-78EB-412C-BDE7-A8B62BC5F962}">
       <formula1>"Identical to v1, Adapted from v1, new"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1" xr:uid="{4FA88F03-C3E1-4A61-AEAF-7DC76A65E608}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J21" xr:uid="{924923CF-D332-45CE-8F54-FF1AFD8AFC9D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J8 J13:J25" xr:uid="{924923CF-D332-45CE-8F54-FF1AFD8AFC9D}">
       <formula1>"DCAT-AP v3, HealthDCAT-AP, DCAT-AP NL, HRI v1, Health and NL"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1" location="terms-publisher" xr:uid="{402E0331-C7FD-45DA-B86E-19A2B3FA6EAF}"/>
-    <hyperlink ref="C21" r:id="rId2" location="terms-title" xr:uid="{BD8E3CB4-1EC3-4556-A50A-36927CAF3730}"/>
-    <hyperlink ref="D11" r:id="rId3" xr:uid="{F932A3CB-8EFE-4EC8-A866-9D436156378C}"/>
-    <hyperlink ref="D12" r:id="rId4" xr:uid="{2EDA5537-713B-44F0-B95C-EC0FE870CDC4}"/>
+    <hyperlink ref="C18" r:id="rId1" location="terms-publisher" xr:uid="{402E0331-C7FD-45DA-B86E-19A2B3FA6EAF}"/>
+    <hyperlink ref="C25" r:id="rId2" location="terms-title" xr:uid="{BD8E3CB4-1EC3-4556-A50A-36927CAF3730}"/>
+    <hyperlink ref="D16" r:id="rId3" xr:uid="{2EDA5537-713B-44F0-B95C-EC0FE870CDC4}"/>
+    <hyperlink ref="D15" r:id="rId4" xr:uid="{F932A3CB-8EFE-4EC8-A866-9D436156378C}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{336390E3-C494-4C9F-BD85-4BDA269484A0}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{34DE2D61-6E14-42AE-9558-EE775580236F}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{97F9B13C-EFF8-43D1-B733-46E03E4766B7}"/>
+    <hyperlink ref="D11" r:id="rId8" xr:uid="{2DAE281E-1462-4EB6-B349-CF7B6187324F}"/>
+    <hyperlink ref="D12" r:id="rId9" xr:uid="{80F65FCA-B4F6-4123-A840-F242D8504306}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8912,14 +9148,14 @@
         <v>216</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>218</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>15</v>
@@ -8938,14 +9174,14 @@
         <v>64</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="37"/>
       <c r="E3" s="38" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F3" s="39" t="s">
         <v>15</v>
@@ -8961,11 +9197,11 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="34" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="34" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D4" s="34"/>
       <c r="E4" s="41"/>
@@ -8973,7 +9209,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="3"/>
@@ -9015,7 +9251,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H6" s="35">
         <v>1</v>
@@ -9025,7 +9261,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="37" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="44" t="s">
@@ -9050,14 +9286,14 @@
         <v>137</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C8" s="34" t="s">
         <v>139</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>25</v>
@@ -9076,14 +9312,14 @@
         <v>187</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>189</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="38" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F9" s="39" t="s">
         <v>25</v>
@@ -9124,14 +9360,14 @@
         <v>160</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C11" s="37" t="s">
         <v>162</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>15</v>
@@ -9150,7 +9386,7 @@
         <v>48</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>50</v>
@@ -9171,10 +9407,10 @@
     </row>
     <row r="13" spans="1:10" ht="43.5">
       <c r="A13" s="37" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C13" s="44" t="s">
         <v>31</v>
@@ -9198,7 +9434,7 @@
         <v>78</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>80</v>
@@ -9207,13 +9443,13 @@
         <v>81</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F14" s="33" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H14" s="35" t="s">
         <v>62</v>
@@ -9223,23 +9459,23 @@
     </row>
     <row r="15" spans="1:10" ht="72">
       <c r="A15" s="37" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="37"/>
       <c r="E15" s="38" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F15" s="39" t="s">
         <v>25</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H15" s="40" t="s">
         <v>27</v>
@@ -9252,14 +9488,14 @@
         <v>204</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C16" s="34" t="s">
         <v>206</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="41" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F16" s="42" t="s">
         <v>25</v>
@@ -9840,10 +10076,10 @@
     </row>
     <row r="2" spans="1:10" ht="60.75" customHeight="1">
       <c r="A2" s="52" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>12</v>
@@ -9858,7 +10094,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H2" s="56">
         <v>1</v>
@@ -9875,7 +10111,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C3" s="57" t="s">
         <v>31</v>
@@ -9902,10 +10138,10 @@
     </row>
     <row r="4" spans="1:10" ht="60.75" customHeight="1">
       <c r="A4" s="52" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>47</v>
@@ -9914,13 +10150,13 @@
         <v>23</v>
       </c>
       <c r="E4" s="121" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F4" s="55" t="s">
         <v>25</v>
       </c>
       <c r="G4" s="55" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H4" s="56" t="s">
         <v>27</v>
@@ -9934,10 +10170,10 @@
     </row>
     <row r="5" spans="1:10" ht="60.75" customHeight="1">
       <c r="A5" s="57" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C5" s="57" t="s">
         <v>50</v>
@@ -10006,7 +10242,7 @@
         <v>25</v>
       </c>
       <c r="G7" s="62" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H7" s="63" t="s">
         <v>27</v>
@@ -10020,10 +10256,10 @@
     </row>
     <row r="8" spans="1:10" ht="60.75" customHeight="1">
       <c r="A8" s="52" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>66</v>
@@ -10050,19 +10286,19 @@
     </row>
     <row r="9" spans="1:10" ht="60.75" customHeight="1">
       <c r="A9" s="57" t="s">
+        <v>380</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>381</v>
+      </c>
+      <c r="C9" s="57" t="s">
         <v>382</v>
-      </c>
-      <c r="B9" s="58" t="s">
-        <v>383</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>384</v>
       </c>
       <c r="D9" s="57" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F9" s="61" t="s">
         <v>25</v>
@@ -10082,13 +10318,13 @@
     </row>
     <row r="10" spans="1:10" ht="60.75" customHeight="1">
       <c r="A10" s="52" t="s">
+        <v>384</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>385</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>386</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>387</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>388</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>23</v>
@@ -10115,7 +10351,7 @@
         <v>267</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C11" s="59" t="s">
         <v>269</v>
@@ -10128,7 +10364,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="62" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H11" s="63" t="s">
         <v>27</v>
@@ -10142,11 +10378,11 @@
     </row>
     <row r="12" spans="1:10" ht="60.75" customHeight="1">
       <c r="A12" s="52" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B12" s="53"/>
       <c r="C12" s="52" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>23</v>
@@ -10170,7 +10406,7 @@
     </row>
     <row r="13" spans="1:10" ht="81.75" customHeight="1">
       <c r="A13" s="57" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B13" s="58"/>
       <c r="C13" s="59" t="s">
@@ -10201,7 +10437,7 @@
         <v>117</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C14" s="52" t="s">
         <v>119</v>
@@ -10228,25 +10464,25 @@
     </row>
     <row r="15" spans="1:10" ht="60.75" customHeight="1">
       <c r="A15" s="57" t="s">
+        <v>393</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="C15" s="57" t="s">
         <v>395</v>
-      </c>
-      <c r="B15" s="58" t="s">
-        <v>396</v>
-      </c>
-      <c r="C15" s="57" t="s">
-        <v>397</v>
       </c>
       <c r="D15" s="57" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="60" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F15" s="117" t="s">
         <v>25</v>
       </c>
       <c r="G15" s="62" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H15" s="63" t="s">
         <v>27</v>
@@ -10288,10 +10524,10 @@
     </row>
     <row r="17" spans="1:10" ht="60.75" customHeight="1">
       <c r="A17" s="57" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C17" s="57" t="s">
         <v>276</v>
@@ -10304,7 +10540,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="62" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H17" s="63">
         <v>1</v>
@@ -10374,10 +10610,10 @@
     </row>
     <row r="20" spans="1:10" ht="60.75" customHeight="1">
       <c r="A20" s="52" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C20" s="52" t="s">
         <v>162</v>
@@ -10404,13 +10640,13 @@
     </row>
     <row r="21" spans="1:10" ht="60.75" customHeight="1">
       <c r="A21" s="57" t="s">
+        <v>401</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>402</v>
+      </c>
+      <c r="C21" s="57" t="s">
         <v>403</v>
-      </c>
-      <c r="B21" s="58" t="s">
-        <v>404</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>405</v>
       </c>
       <c r="D21" s="57" t="s">
         <v>23</v>
@@ -10434,10 +10670,10 @@
     </row>
     <row r="22" spans="1:10" ht="60.75" customHeight="1">
       <c r="A22" s="52" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C22" s="52" t="s">
         <v>213</v>
@@ -10446,7 +10682,7 @@
         <v>23</v>
       </c>
       <c r="E22" s="65" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F22" s="67" t="s">
         <v>15</v>
@@ -10469,7 +10705,7 @@
         <v>216</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C23" s="59" t="s">
         <v>218</v>
@@ -10984,7 +11220,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="75" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B2" s="76"/>
       <c r="C2" s="75" t="s">
@@ -10998,7 +11234,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="78" t="s">
-        <v>312</v>
+        <v>409</v>
       </c>
       <c r="H2" s="79" t="s">
         <v>27</v>
@@ -11010,13 +11246,13 @@
     </row>
     <row r="3" spans="1:10" ht="101.25">
       <c r="A3" s="81" t="s">
+        <v>410</v>
+      </c>
+      <c r="B3" s="82" t="s">
         <v>411</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="C3" s="81" t="s">
         <v>412</v>
-      </c>
-      <c r="C3" s="81" t="s">
-        <v>413</v>
       </c>
       <c r="D3" s="81" t="s">
         <v>23</v>
@@ -11043,7 +11279,7 @@
         <v>105</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C4" s="75" t="s">
         <v>107</v>
@@ -11065,24 +11301,24 @@
         <v>58</v>
       </c>
       <c r="J4" s="80" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="29.25">
       <c r="A5" s="123" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="123" t="s">
         <v>417</v>
-      </c>
-      <c r="C5" s="123" t="s">
-        <v>418</v>
       </c>
       <c r="D5" s="57" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="124" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F5" s="125" t="s">
         <v>15</v>
@@ -11105,7 +11341,7 @@
         <v>219</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C6" s="129" t="s">
         <v>221</v>
@@ -11114,7 +11350,7 @@
         <v>169</v>
       </c>
       <c r="E6" s="88" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F6" s="89" t="s">
         <v>25</v>
@@ -11134,13 +11370,13 @@
     </row>
     <row r="7" spans="1:10" ht="57.75">
       <c r="A7" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>423</v>
-      </c>
       <c r="C7" s="123" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D7" s="123" t="s">
         <v>23</v>
@@ -11841,13 +12077,13 @@
     </row>
     <row r="2" spans="1:10" ht="57.75">
       <c r="A2" s="75" t="s">
+        <v>423</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>422</v>
+      </c>
+      <c r="C2" s="129" t="s">
         <v>424</v>
-      </c>
-      <c r="B2" s="76" t="s">
-        <v>423</v>
-      </c>
-      <c r="C2" s="129" t="s">
-        <v>425</v>
       </c>
       <c r="D2" s="75" t="s">
         <v>23</v>
@@ -11871,13 +12107,13 @@
     </row>
     <row r="3" spans="1:10" ht="29.25">
       <c r="A3" s="81" t="s">
+        <v>425</v>
+      </c>
+      <c r="B3" s="82" t="s">
         <v>426</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="C3" s="81" t="s">
         <v>427</v>
-      </c>
-      <c r="C3" s="81" t="s">
-        <v>428</v>
       </c>
       <c r="D3" s="131" t="s">
         <v>23</v>
@@ -11901,13 +12137,13 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="75" t="s">
+        <v>428</v>
+      </c>
+      <c r="B4" s="76" t="s">
         <v>429</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="C4" s="75" t="s">
         <v>430</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>431</v>
       </c>
       <c r="D4" s="75" t="s">
         <v>23</v>
@@ -11917,7 +12153,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="78" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H4" s="79">
         <v>1</v>
@@ -12641,10 +12877,10 @@
     </row>
     <row r="2" spans="1:10" ht="43.5">
       <c r="A2" s="76" t="s">
+        <v>431</v>
+      </c>
+      <c r="B2" s="94" t="s">
         <v>432</v>
-      </c>
-      <c r="B2" s="94" t="s">
-        <v>433</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="96" t="s">
@@ -12655,7 +12891,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="97" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H2" s="80">
         <v>1</v>
@@ -12669,10 +12905,10 @@
     </row>
     <row r="3" spans="1:10" ht="72.75">
       <c r="A3" s="82" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" s="98" t="s">
         <v>435</v>
-      </c>
-      <c r="B3" s="98" t="s">
-        <v>436</v>
       </c>
       <c r="C3" s="81"/>
       <c r="D3" s="83" t="s">
@@ -12683,7 +12919,7 @@
         <v>15</v>
       </c>
       <c r="G3" s="85" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H3" s="87">
         <v>1</v>
@@ -13354,13 +13590,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="95" t="s">
+        <v>437</v>
+      </c>
+      <c r="B2" s="76" t="s">
         <v>438</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="C2" s="132" t="s">
         <v>439</v>
-      </c>
-      <c r="C2" s="132" t="s">
-        <v>440</v>
       </c>
       <c r="D2" s="95" t="s">
         <v>23</v>
@@ -13384,13 +13620,13 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="81" t="s">
+        <v>440</v>
+      </c>
+      <c r="B3" s="82" t="s">
         <v>441</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="C3" s="133" t="s">
         <v>442</v>
-      </c>
-      <c r="C3" s="133" t="s">
-        <v>443</v>
       </c>
       <c r="D3" s="81" t="s">
         <v>23</v>

</xml_diff>